<commit_message>
Commit syun Branch changes
</commit_message>
<xml_diff>
--- a/Troy.Web/Troy.Web/App_Data/ExcelFiles/lasttesting.xlsx
+++ b/Troy.Web/Troy.Web/App_Data/ExcelFiles/lasttesting.xlsx
@@ -911,7 +911,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,9 +958,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>15</v>
-      </c>
+      <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>